<commit_message>
Intro to computer Science Excel lab.xlsx
</commit_message>
<xml_diff>
--- a/Intro to computer Science Excel lab.xlsx
+++ b/Intro to computer Science Excel lab.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bda7604644b7074f/Desktop/ExcelLab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alinj\OneDrive\Desktop\ExcelLab\labExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38FC59DE-8B95-47B1-A785-1D905BEB5C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{38FC59DE-8B95-47B1-A785-1D905BEB5C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0042BA1D-7D23-4D76-AEEF-CB389EF034B9}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="3105" windowWidth="18000" windowHeight="12735" activeTab="1" xr2:uid="{8741ECEE-441E-4C82-B611-19D77D8C299D}"/>
+    <workbookView xWindow="3675" yWindow="8010" windowWidth="18000" windowHeight="12735" xr2:uid="{8741ECEE-441E-4C82-B611-19D77D8C299D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Country</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t xml:space="preserve">in conclusion we can see that Saudi Arabia has been the leading country In emitting CO2 and poluting the world, mainly due to the oil factories they have. </t>
+  </si>
+  <si>
+    <t>Ali Alnajjar</t>
+  </si>
+  <si>
+    <t>date: 10/03/2020</t>
   </si>
 </sst>
 </file>
@@ -1628,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28100576-7808-47B1-AAAB-C2D0FFB5634E}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1650,24 +1656,30 @@
     <col min="12" max="19" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1678,7 +1690,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" s="4"/>
       <c r="E6" s="4">
         <v>1</v>
@@ -1690,7 +1702,7 @@
         <v>18.48</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" s="4"/>
       <c r="E7" s="4">
         <v>2</v>
@@ -1702,7 +1714,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" s="4"/>
       <c r="E8" s="4">
         <v>3</v>
@@ -1714,7 +1726,7 @@
         <v>16.920000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" s="4"/>
       <c r="E9" s="4">
         <v>4</v>
@@ -1726,7 +1738,7 @@
         <v>16.559999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" s="4"/>
       <c r="E10" s="4">
         <v>5</v>
@@ -1738,7 +1750,7 @@
         <v>15.32</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" s="4"/>
       <c r="E11" s="4">
         <v>6</v>
@@ -1750,7 +1762,7 @@
         <v>12.89</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1">
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="4"/>
       <c r="E12" s="4">
         <v>7</v>
@@ -1762,7 +1774,7 @@
         <v>11.74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1">
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="4"/>
       <c r="E13" s="4">
         <v>8</v>
@@ -1774,7 +1786,7 @@
         <v>9.1300000000000008</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1">
+    <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="4"/>
       <c r="E14" s="4">
         <v>9</v>
@@ -1786,7 +1798,7 @@
         <v>9.1199999999999992</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" s="4"/>
       <c r="E15" s="4">
         <v>10</v>
@@ -1798,7 +1810,7 @@
         <v>9.08</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="4"/>
       <c r="E16" s="4">
         <v>11</v>
@@ -2078,7 +2090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC540C66-A813-4159-8314-9C3454149059}">
   <dimension ref="A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>

</xml_diff>